<commit_message>
create data for tc02
</commit_message>
<xml_diff>
--- a/com.tutorial.Automation.Ecomercesite/src/test/resources/Data/DataFile.xlsx
+++ b/com.tutorial.Automation.Ecomercesite/src/test/resources/Data/DataFile.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10335"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10335" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TC01_TestLogin" sheetId="5" r:id="rId1"/>
+    <sheet name="TC02_TestSendARequest" sheetId="6" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="birth_day">#REF!</definedName>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Password</t>
   </si>
@@ -43,13 +44,58 @@
   </si>
   <si>
     <t>123456789</t>
+  </si>
+  <si>
+    <t>Subject header</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>OrderID</t>
+  </si>
+  <si>
+    <t>Attached</t>
+  </si>
+  <si>
+    <t>FileName</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>Subject Source</t>
+  </si>
+  <si>
+    <t>Customer service</t>
+  </si>
+  <si>
+    <t>Webmaster</t>
+  </si>
+  <si>
+    <t>user10@gmail.com</t>
+  </si>
+  <si>
+    <t>Yes/No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>cong hoa xa hoi chu nghia viet nam</t>
+  </si>
+  <si>
+    <t>C:/testing.txt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,6 +110,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -87,10 +139,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -374,7 +427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -406,4 +459,100 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="12" max="12" width="19.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2">
+        <v>1100012</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2">
+      <formula1>$L$2:$L$3</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2">
+      <formula1>$M$2:$M$3</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add test case 04
</commit_message>
<xml_diff>
--- a/com.tutorial.Automation.Ecomercesite/src/test/resources/Data/DataFile.xlsx
+++ b/com.tutorial.Automation.Ecomercesite/src/test/resources/Data/DataFile.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WorkingProjects\workspace\Ecommercialwebsite\com.tutorial.Automation.Ecomercesite\src\test\resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WorkingProjects\workspace\Ecommercialwebsite\EcommercialProject\com.tutorial.Automation.Ecomercesite\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10335" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10335" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TC01_TestLogin" sheetId="5" r:id="rId1"/>
     <sheet name="TC02_TestSendARequest" sheetId="6" r:id="rId2"/>
     <sheet name="TC03_TestSignUpAnAccount" sheetId="7" r:id="rId3"/>
+    <sheet name="TC04_SearchProduct" sheetId="8" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="birth_day">#REF!</definedName>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t>Password</t>
   </si>
@@ -132,12 +133,33 @@
   </si>
   <si>
     <t>year</t>
+  </si>
+  <si>
+    <t>Search Item</t>
+  </si>
+  <si>
+    <t>Blouse</t>
+  </si>
+  <si>
+    <t>Image source</t>
+  </si>
+  <si>
+    <t>http://automationpractice.com/img/p/7/7-home_default.jpg</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>$27.00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -182,11 +204,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -604,7 +628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
@@ -1431,4 +1455,49 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="4"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add run muiltiple file at once
</commit_message>
<xml_diff>
--- a/com.tutorial.Automation.Ecomercesite/src/test/resources/Data/DataFile.xlsx
+++ b/com.tutorial.Automation.Ecomercesite/src/test/resources/Data/DataFile.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10335" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10335" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TC01_TestLogin" sheetId="5" r:id="rId1"/>
@@ -628,7 +628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q120"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
@@ -1461,7 +1461,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>